<commit_message>
Change AI casting long range abilities behavior & improve QOL features
</commit_message>
<xml_diff>
--- a/Assets/Test/Numbers.xlsx
+++ b/Assets/Test/Numbers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program\unity\Project\LastDevotion\Assets\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E23F9F-91DD-42EA-99D7-9D0EA597D515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B1C29E-B7C3-446C-ACE8-53BD3E282091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>RubyRose</t>
   </si>
@@ -51,6 +51,9 @@
     <t>Soul Ledger: Each strike brands the enemy with a death mark, storing (5 + 0.1 * reflex)% of their max HP per hit.
 The mark stacks infinitely.
 When the enemy’s HP falls below the total stored mark value, she instantly dashes near them, cleaving with her scythe for damage equal to the stored amount.</t>
+  </si>
+  <si>
+    <t>JapaneseSamurai</t>
   </si>
 </sst>
 </file>
@@ -95,7 +98,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -377,14 +380,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="14.88671875" customWidth="1"/>
     <col min="2" max="2" width="47" customWidth="1"/>
   </cols>
   <sheetData>
@@ -415,6 +419,8 @@
         <v>1000</v>
       </c>
       <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="119.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -433,6 +439,24 @@
         <v>3</v>
       </c>
       <c r="F3" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1">
+        <v>50</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="F4" s="1">
         <v>100</v>
       </c>
     </row>

</xml_diff>